<commit_message>
Comit to basic learning
</commit_message>
<xml_diff>
--- a/code/销售额统计表.xlsx
+++ b/code/销售额统计表.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\工作\1、创作中\Excel VBA应用与技巧大全（新）\实例文件\第1章\原始文件\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\Excel VBA应用与技巧大全\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18ABC56-53CD-4E4B-913B-4D8B77790003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB4C0D2-8498-4B3A-923C-122AAC02ACAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="4305" activeTab="1" xr2:uid="{D5968162-9AED-4B28-A1FA-228FFE6C2719}"/>
+    <workbookView xWindow="14625" yWindow="1005" windowWidth="21600" windowHeight="13155" activeTab="1" xr2:uid="{D5968162-9AED-4B28-A1FA-228FFE6C2719}"/>
   </bookViews>
   <sheets>
     <sheet name="1月" sheetId="1" r:id="rId1"/>
     <sheet name="2月" sheetId="2" r:id="rId2"/>
     <sheet name="3月" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23110,7 +23110,7 @@
   <dimension ref="A1:F1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>